<commit_message>
probe el excel del roro
</commit_message>
<xml_diff>
--- a/Productos.xlsx
+++ b/Productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -34,7 +34,7 @@
     <t>prueba</t>
   </si>
   <si>
-    <t>0.0</t>
+    <t>5000.0</t>
   </si>
   <si>
     <t>inactivo</t>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>80000.0</t>
-  </si>
-  <si>
-    <t>flavio</t>
   </si>
 </sst>
 </file>
@@ -405,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -513,23 +510,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>10000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
agregando aviso bajo stock
</commit_message>
<xml_diff>
--- a/Productos.xlsx
+++ b/Productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Nombre</t>
   </si>
@@ -31,40 +31,31 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>5000.0</t>
+    <t>vodka negro</t>
+  </si>
+  <si>
+    <t>8000.0</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>Destilados</t>
+  </si>
+  <si>
+    <t>vodka blanco</t>
+  </si>
+  <si>
+    <t>8900.0</t>
+  </si>
+  <si>
+    <t>jagger</t>
+  </si>
+  <si>
+    <t>10000.0</t>
   </si>
   <si>
     <t>inactivo</t>
-  </si>
-  <si>
-    <t>Cervezas</t>
-  </si>
-  <si>
-    <t>vodka negro</t>
-  </si>
-  <si>
-    <t>8000.0</t>
-  </si>
-  <si>
-    <t>activo</t>
-  </si>
-  <si>
-    <t>Destilados</t>
-  </si>
-  <si>
-    <t>vodka blanco</t>
-  </si>
-  <si>
-    <t>8900.0</t>
-  </si>
-  <si>
-    <t>jagger</t>
-  </si>
-  <si>
-    <t>10000.0</t>
   </si>
   <si>
     <t>jack daniels</t>
@@ -402,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -433,7 +424,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -450,64 +441,47 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrego funciones para senalizar iconos , y el volver atras de movimiento instalar pip install tkinter-tooltip
</commit_message>
<xml_diff>
--- a/Productos.xlsx
+++ b/Productos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>80000.0</t>
+  </si>
+  <si>
+    <t>jose</t>
+  </si>
+  <si>
+    <t>20000.0</t>
+  </si>
+  <si>
+    <t>Vinos</t>
   </si>
 </sst>
 </file>
@@ -393,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -484,6 +493,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>